<commit_message>
Cambios a nombres de campos en tabla maratones
</commit_message>
<xml_diff>
--- a/BasesDatos/BDs.xlsx
+++ b/BasesDatos/BDs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="18855" windowHeight="8970"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="18855" windowHeight="8970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mexflix" sheetId="1" r:id="rId1"/>
@@ -833,9 +833,6 @@
     <t>race_date</t>
   </si>
   <si>
-    <t>since</t>
-  </si>
-  <si>
     <t>TCS New York City Marathon</t>
   </si>
   <si>
@@ -942,6 +939,9 @@
   </si>
   <si>
     <t xml:space="preserve">Maratón de la Ciudad de México Telcel </t>
+  </si>
+  <si>
+    <t>since_year</t>
   </si>
 </sst>
 </file>
@@ -1328,7 +1328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -3558,8 +3558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L200"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3568,7 +3568,7 @@
     <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="48.42578125" bestFit="1" customWidth="1"/>
@@ -3644,7 +3644,7 @@
         <v>269</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>272</v>
+        <v>308</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>271</v>
@@ -3667,28 +3667,28 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>106</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F7" s="1">
         <v>2007</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K7" s="3">
         <v>1</v>
@@ -3702,28 +3702,28 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F8" s="1">
         <v>1897</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K8" s="3">
         <v>2</v>
@@ -3737,28 +3737,28 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>156</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F9" s="1">
         <v>1981</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K9" s="3">
         <v>3</v>
@@ -3772,28 +3772,28 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F10" s="1">
         <v>1974</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K10" s="3">
         <v>4</v>
@@ -3807,28 +3807,28 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F11" s="1">
         <v>1977</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K11" s="3">
         <v>5</v>
@@ -3842,28 +3842,28 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F12" s="1">
         <v>1970</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>276</v>
-      </c>
       <c r="I12" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K12" s="3">
         <v>6</v>
@@ -3877,28 +3877,28 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>131</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F13" s="1">
         <v>1983</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>305</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>306</v>
       </c>
       <c r="K13" s="3">
         <v>7</v>

</xml_diff>